<commit_message>
updated cocktail_hyper_alpha experiment: 0.1 and 1.0 of BFact and noLT
</commit_message>
<xml_diff>
--- a/notes/experiment_log.xlsx
+++ b/notes/experiment_log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>kernel=Gaussian</t>
   </si>
@@ -102,21 +102,6 @@
     <t>&lt;results/cockail_s16_m12/kernel/&gt;</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">{a/b}_alpha={0.1, 1.0} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;{0.01, 5.0}&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>kernel={gaussian,cauchy,laplace}</t>
   </si>
   <si>
@@ -136,6 +121,33 @@
   </si>
   <si>
     <t>script=exp_hyper_alpha_plus_lambda1p6() ; NOTE: a bit hacky, includes hyper_alpha</t>
+  </si>
+  <si>
+    <t>{a/b}_alpha={0.01, 0.1, 1.0, 5.0}</t>
+  </si>
+  <si>
+    <t>{a/b}_h={0.01, 0.1, 1.0, 5.0}</t>
+  </si>
+  <si>
+    <t>lambda=1.6</t>
+  </si>
+  <si>
+    <t>cauchy</t>
+  </si>
+  <si>
+    <t>results/continuous_latent_syn/block_diag40/block_diag40_s2</t>
+  </si>
+  <si>
+    <t>data_source=block_diag40_s2</t>
+  </si>
+  <si>
+    <t>script=</t>
+  </si>
+  <si>
+    <t>LT only</t>
+  </si>
+  <si>
+    <t>LT_hdp_hmm_w0_lambda1_cauchy</t>
   </si>
 </sst>
 </file>
@@ -219,8 +231,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -326,7 +344,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -375,6 +393,9 @@
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -423,6 +444,9 @@
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -752,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N41"/>
+  <dimension ref="B2:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -765,7 +789,7 @@
     <col min="6" max="6" width="38.83203125" customWidth="1"/>
     <col min="8" max="8" width="38" customWidth="1"/>
     <col min="10" max="10" width="32.6640625" customWidth="1"/>
-    <col min="12" max="12" width="32.1640625" customWidth="1"/>
+    <col min="12" max="12" width="52.33203125" customWidth="1"/>
     <col min="14" max="14" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -798,19 +822,19 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
         <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="J5" t="s">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
         <v>5</v>
@@ -862,18 +886,18 @@
     </row>
     <row r="12" spans="2:14">
       <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" t="s">
         <v>33</v>
-      </c>
-      <c r="N12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:14">
       <c r="D13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:14">
@@ -881,7 +905,7 @@
         <v>3</v>
       </c>
       <c r="N14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:14">
@@ -906,7 +930,7 @@
     </row>
     <row r="16" spans="2:14">
       <c r="D16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N16" t="s">
         <v>4</v>
@@ -914,7 +938,7 @@
     </row>
     <row r="17" spans="2:14">
       <c r="N17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:14">
@@ -974,6 +998,9 @@
       <c r="H25" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="L25" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="26" spans="2:14">
       <c r="D26" s="5" t="s">
@@ -984,67 +1011,108 @@
       </c>
       <c r="H26" s="5" t="s">
         <v>21</v>
+      </c>
+      <c r="L26" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="2:14">
       <c r="D27" s="5"/>
       <c r="F27" s="5"/>
       <c r="H27" s="5"/>
+      <c r="L27" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="28" spans="2:14">
       <c r="D28" s="5"/>
       <c r="F28" s="5"/>
       <c r="H28" s="5"/>
+      <c r="L28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14">
+      <c r="D29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="L29" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="30" spans="2:14">
-      <c r="B30" s="3" t="s">
-        <v>12</v>
+      <c r="D30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="L30" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:14">
-      <c r="D31" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>21</v>
+      <c r="D31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="L31" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="2:14">
       <c r="D32" s="5"/>
       <c r="F32" s="5"/>
       <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="2:8">
-      <c r="D33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="L32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="35" spans="2:8">
-      <c r="B35" s="3" t="s">
+      <c r="D35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="D36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="D37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="2:8">
-      <c r="B36" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8">
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="2:8">
-      <c r="B38" s="5"/>
-    </row>
     <row r="40" spans="2:8">
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="5"/>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="2:8">
-      <c r="B41" s="5" t="s">
+    <row r="45" spans="2:8">
+      <c r="B45" s="5" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding cocktail_hyper_alpha experiment Sticky and StickyLT
</commit_message>
<xml_diff>
--- a/notes/experiment_log.xlsx
+++ b/notes/experiment_log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>kernel=Gaussian</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>LT_hdp_hmm_w0_lambda1_cauchy</t>
+  </si>
+  <si>
+    <t>sticky: beta prior</t>
   </si>
 </sst>
 </file>
@@ -779,7 +782,7 @@
   <dimension ref="B2:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -797,6 +800,9 @@
       <c r="B2" t="s">
         <v>17</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="3" spans="2:14">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
hyper_gamma experiment with a,b={0.01, 5} X {BFact, LT, noLT, Sticky, StickyLT} X 5-reps
</commit_message>
<xml_diff>
--- a/notes/experiment_log.xlsx
+++ b/notes/experiment_log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26660" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="0" windowWidth="26660" windowHeight="17000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>kernel=Gaussian</t>
   </si>
@@ -75,9 +75,6 @@
     <t>legend:</t>
   </si>
   <si>
-    <t>{a/b}_gamma={0.01, 0.1, 1.0, 5.0}</t>
-  </si>
-  <si>
     <t>&lt;choose diff lambdas?&gt;</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>&lt;results/cockail_s16_m12_CHiME/hyper_alpha&gt;</t>
   </si>
   <si>
-    <t>&lt;results/cockail_s16_m12/hyper_gamma/&gt;</t>
-  </si>
-  <si>
     <t>&lt;results/cockail_s16_m12/hyper_h/&gt;</t>
   </si>
   <si>
@@ -150,7 +144,34 @@
     <t>LT_hdp_hmm_w0_lambda1_cauchy</t>
   </si>
   <si>
-    <t>sticky: beta prior</t>
+    <t>{a/b}_alpha={0.01, 5.0}</t>
+  </si>
+  <si>
+    <t>{Sticky, StickyLT}  : with uniform beta prior to sticky param</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{a/b}_gamma={0.01,  5.0}   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TODO: 0.1, 1.0,</t>
+    </r>
+  </si>
+  <si>
+    <t>script=exp_hyper_gamma()</t>
+  </si>
+  <si>
+    <t>restuls/cocktail_s16_m12/hyper_gamma/</t>
+  </si>
+  <si>
+    <t>{BFact, LT, noLT, Sticky, StickyLT}</t>
   </si>
 </sst>
 </file>
@@ -234,8 +255,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -347,7 +384,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -399,6 +436,14 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -450,6 +495,14 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -779,37 +832,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N45"/>
+  <dimension ref="B2:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="33.5" customWidth="1"/>
     <col min="4" max="4" width="52.6640625" customWidth="1"/>
-    <col min="6" max="6" width="38.83203125" customWidth="1"/>
-    <col min="8" max="8" width="38" customWidth="1"/>
-    <col min="10" max="10" width="32.6640625" customWidth="1"/>
-    <col min="12" max="12" width="52.33203125" customWidth="1"/>
-    <col min="14" max="14" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="52.6640625" customWidth="1"/>
+    <col min="8" max="8" width="45.1640625" customWidth="1"/>
+    <col min="10" max="10" width="38" customWidth="1"/>
+    <col min="12" max="12" width="32.6640625" customWidth="1"/>
+    <col min="14" max="14" width="52.33203125" customWidth="1"/>
+    <col min="16" max="16" width="73.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:16">
       <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:16">
       <c r="B3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:16">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -817,56 +872,64 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14">
+    </row>
+    <row r="5" spans="2:16">
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" t="s">
         <v>0</v>
       </c>
-      <c r="L5" t="s">
-        <v>27</v>
-      </c>
       <c r="N5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:16">
       <c r="B6" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16">
       <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16">
       <c r="B8" s="4"/>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:16">
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:14">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="2:16">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -874,252 +937,311 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>21</v>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:16">
       <c r="D12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16">
       <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="N13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
       <c r="D14" t="s">
         <v>3</v>
       </c>
-      <c r="N14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14">
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
       <c r="D15" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" s="4" t="s">
+      <c r="P15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
+      <c r="D16" t="s">
         <v>26</v>
       </c>
-      <c r="N15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14">
-      <c r="D16" t="s">
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
+        <v>45</v>
+      </c>
+      <c r="P16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16">
+      <c r="P17" t="s">
         <v>28</v>
       </c>
-      <c r="N16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14">
-      <c r="N17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14">
+    </row>
+    <row r="19" spans="2:16">
       <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="2:16">
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P20" s="5"/>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="D21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="5"/>
-    </row>
-    <row r="21" spans="2:14">
-      <c r="D21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="5"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
       <c r="H21" s="5"/>
       <c r="J21" s="5"/>
       <c r="L21" s="5"/>
       <c r="N21" s="5"/>
-    </row>
-    <row r="22" spans="2:14">
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" spans="2:16">
       <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="H22" s="5"/>
       <c r="J22" s="5"/>
       <c r="L22" s="5"/>
       <c r="N22" s="5"/>
-    </row>
-    <row r="25" spans="2:14">
+      <c r="P22" s="5"/>
+    </row>
+    <row r="25" spans="2:16">
       <c r="B25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
       <c r="H25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14">
+        <v>18</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16">
       <c r="D26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
       <c r="H26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14">
+        <v>20</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16">
       <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="L27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14">
+      <c r="J27" s="5"/>
+      <c r="N27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16">
       <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="H28" s="5"/>
-      <c r="L28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14">
+      <c r="J28" s="5"/>
+      <c r="N28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16">
       <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="H29" s="5"/>
-      <c r="L29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14">
+      <c r="J29" s="5"/>
+      <c r="N29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16">
       <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="H30" s="5"/>
-      <c r="L30" t="s">
+      <c r="J30" s="5"/>
+      <c r="N30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:14">
+    <row r="31" spans="2:16">
       <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="H31" s="5"/>
-      <c r="L31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14">
+      <c r="J31" s="5"/>
+      <c r="N31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16">
       <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="H32" s="5"/>
-      <c r="L32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8">
+      <c r="J32" s="5"/>
+      <c r="N32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
       <c r="B34" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="2:10">
       <c r="D35" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
       <c r="H35" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8">
+        <v>20</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
       <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="2:8">
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="2:10">
       <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="H37" s="5"/>
-    </row>
-    <row r="39" spans="2:8">
+      <c r="J37" s="5"/>
+    </row>
+    <row r="39" spans="2:10">
       <c r="B39" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="2:8">
+    <row r="40" spans="2:10">
       <c r="B40" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
       <c r="B41" s="5"/>
     </row>
-    <row r="42" spans="2:8">
+    <row r="42" spans="2:10">
       <c r="B42" s="5"/>
     </row>
-    <row r="44" spans="2:8">
+    <row r="44" spans="2:10">
       <c r="B44" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="2:10">
       <c r="B45" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
music21 Bach chorale preprocessing in-progress
</commit_message>
<xml_diff>
--- a/notes/experiment_log.xlsx
+++ b/notes/experiment_log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>kernel=Gaussian</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>{BFact, LT, noLT, Sticky, StickyLT}</t>
+  </si>
+  <si>
+    <t>(sticky with uniform beta prior)</t>
   </si>
 </sst>
 </file>
@@ -834,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -911,6 +914,9 @@
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" s="5" t="s">

</xml_diff>

<commit_message>
version 1 of generating music21_bach_chorales hamlet data complete
</commit_message>
<xml_diff>
--- a/notes/experiment_log.xlsx
+++ b/notes/experiment_log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>kernel=Gaussian</t>
   </si>
@@ -87,9 +87,6 @@
     <t>&lt;results/cockail_s16_m12_CHiME/hyper_alpha&gt;</t>
   </si>
   <si>
-    <t>&lt;results/cockail_s16_m12/hyper_h/&gt;</t>
-  </si>
-  <si>
     <t>&lt;results/cockail_s16_m12/lambda/&gt;</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
   </si>
   <si>
     <t>{a/b}_alpha={0.01, 0.1, 1.0, 5.0}</t>
-  </si>
-  <si>
-    <t>{a/b}_h={0.01, 0.1, 1.0, 5.0}</t>
   </si>
   <si>
     <t>lambda=1.6</t>
@@ -175,6 +169,12 @@
   </si>
   <si>
     <t>(sticky with uniform beta prior)</t>
+  </si>
+  <si>
+    <t>restuls/cocktail_s16_m12/hyper_h/</t>
+  </si>
+  <si>
+    <t>script=exp_hyper_h()</t>
   </si>
 </sst>
 </file>
@@ -258,8 +258,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -387,7 +393,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -447,6 +453,9 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -506,6 +515,9 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -837,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -848,7 +860,7 @@
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="52.6640625" customWidth="1"/>
     <col min="8" max="8" width="45.1640625" customWidth="1"/>
-    <col min="10" max="10" width="38" customWidth="1"/>
+    <col min="10" max="10" width="45.33203125" customWidth="1"/>
     <col min="12" max="12" width="32.6640625" customWidth="1"/>
     <col min="14" max="14" width="52.33203125" customWidth="1"/>
     <col min="16" max="16" width="73.6640625" customWidth="1"/>
@@ -875,10 +887,10 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s">
         <v>7</v>
@@ -889,22 +901,22 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
         <v>41</v>
       </c>
-      <c r="H5" t="s">
-        <v>43</v>
-      </c>
       <c r="J5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="L5" t="s">
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P5" t="s">
         <v>5</v>
@@ -915,7 +927,7 @@
         <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:16">
@@ -949,8 +961,8 @@
       <c r="H11" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>20</v>
+      <c r="J11" t="s">
+        <v>16</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>20</v>
@@ -964,31 +976,37 @@
     </row>
     <row r="12" spans="2:16">
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P12" t="s">
         <v>30</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:16">
       <c r="D13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>26</v>
       </c>
       <c r="P13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:16">
@@ -1001,8 +1019,11 @@
       <c r="H14" t="s">
         <v>3</v>
       </c>
+      <c r="J14" t="s">
+        <v>3</v>
+      </c>
       <c r="P14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:16">
@@ -1015,14 +1036,14 @@
       <c r="H15" t="s">
         <v>4</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="P15" t="s">
         <v>3</v>
@@ -1030,13 +1051,16 @@
     </row>
     <row r="16" spans="2:16">
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="J16" t="s">
+        <v>46</v>
       </c>
       <c r="P16" t="s">
         <v>4</v>
@@ -1044,7 +1068,7 @@
     </row>
     <row r="17" spans="2:16">
       <c r="P17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:16">
@@ -1113,7 +1137,7 @@
         <v>18</v>
       </c>
       <c r="N25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="2:16">
@@ -1129,7 +1153,7 @@
         <v>20</v>
       </c>
       <c r="N26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="2:16">
@@ -1139,7 +1163,7 @@
       <c r="H27" s="5"/>
       <c r="J27" s="5"/>
       <c r="N27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="2:16">
@@ -1149,7 +1173,7 @@
       <c r="H28" s="5"/>
       <c r="J28" s="5"/>
       <c r="N28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:16">
@@ -1159,7 +1183,7 @@
       <c r="H29" s="5"/>
       <c r="J29" s="5"/>
       <c r="N29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:16">
@@ -1179,7 +1203,7 @@
       <c r="H31" s="5"/>
       <c r="J31" s="5"/>
       <c r="N31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="2:16">
@@ -1189,7 +1213,7 @@
       <c r="H32" s="5"/>
       <c r="J32" s="5"/>
       <c r="N32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="2:10">

</xml_diff>